<commit_message>
Updated formatting of 3d print doc
</commit_message>
<xml_diff>
--- a/fdm/filesandsettings.xlsx
+++ b/fdm/filesandsettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\kinetic-display\fdm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759E18CB-DA51-48D2-87D7-DAAEE7D1658B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03277F9-4F2C-48ED-8D4A-8CACD9BB9044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{D0B1DBA1-9AFF-44C2-A8AD-2E890C375429}"/>
   </bookViews>
@@ -41,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="115">
-  <si>
-    <t>Material</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="114">
   <si>
     <t>Color</t>
   </si>
@@ -268,24 +265,15 @@
     <t>Digit 7-segment G</t>
   </si>
   <si>
-    <t>stl</t>
-  </si>
-  <si>
     <t>Kinetic display stand, buck converter mounts, and powerbank PCB mount</t>
   </si>
   <si>
-    <t>stl quantity</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
     <t>PLA Matte</t>
   </si>
   <si>
-    <t>Build Plate</t>
-  </si>
-  <si>
     <t>textured</t>
   </si>
   <si>
@@ -304,21 +292,9 @@
     <t>nylon-smooth-black</t>
   </si>
   <si>
-    <t>Top Surface Ironing</t>
-  </si>
-  <si>
     <t>Detect Thin Walls</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>per unit (g)</t>
-  </si>
-  <si>
-    <t>total (g)</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
@@ -376,9 +352,6 @@
     <t>monotonic</t>
   </si>
   <si>
-    <t>Fill Density</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -386,6 +359,30 @@
   </si>
   <si>
     <t>Sum of total (g)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Plate</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Ironing</t>
+  </si>
+  <si>
+    <t>Total (g)</t>
+  </si>
+  <si>
+    <t>Per Unit (g)</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -1159,21 +1156,27 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B34015F8-2D9A-4B55-BF90-5F33C7A38316}" name="Table1" displayName="Table1" ref="A1:M26" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M26" xr:uid="{B34015F8-2D9A-4B55-BF90-5F33C7A38316}"/>
+  <autoFilter ref="A1:M26" xr:uid="{B34015F8-2D9A-4B55-BF90-5F33C7A38316}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="tpu-smooth-black"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{F9BBA264-6B03-4C06-B16C-6C3A9D230F1B}" name="3mf" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{402B400E-7457-4E87-AD2C-315243B5053D}" name="stl" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{B24AFC94-BF77-44E9-806A-A82AF3C36BF7}" name="description" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{E686FE53-EC6F-411F-BCCE-8620E78B08FE}" name="stl quantity" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{22218451-E857-437D-93CF-2C6BDF91A9F6}" name="per unit (g)" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{44D76CB5-67A6-492F-989F-88F774A32071}" name="total (g)" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{402B400E-7457-4E87-AD2C-315243B5053D}" name="STL" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B24AFC94-BF77-44E9-806A-A82AF3C36BF7}" name="Description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E686FE53-EC6F-411F-BCCE-8620E78B08FE}" name="Quantity" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{22218451-E857-437D-93CF-2C6BDF91A9F6}" name="Per Unit (g)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{44D76CB5-67A6-492F-989F-88F774A32071}" name="Total (g)" dataDxfId="7">
       <calculatedColumnFormula>D2*E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{134E0C4B-A950-4699-9906-A5112792339D}" name="Material" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{134E0C4B-A950-4699-9906-A5112792339D}" name="Type" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{17747416-B343-422A-B64A-390839F424EB}" name="Color" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{7780B91F-DE55-4D83-8C60-A0FF0E6A9076}" name="Build Plate" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{86830753-8A8D-4773-8D8E-E7CF47D0566D}" name="Fill Density" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{33F1EAB2-CFCB-42B0-973A-82A906131ABC}" name="Top Surface Ironing" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{7780B91F-DE55-4D83-8C60-A0FF0E6A9076}" name="Plate" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{86830753-8A8D-4773-8D8E-E7CF47D0566D}" name="Density" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{33F1EAB2-CFCB-42B0-973A-82A906131ABC}" name="Ironing" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{561A42C3-F5B4-4A48-B680-C1CE7E3FEFE0}" name="Detect Thin Walls" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{70CBC5D4-9212-4385-B68D-805E278FA576}" name="Top and bottom shell pattern" dataDxfId="0"/>
   </tableColumns>
@@ -1500,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FA87BA-1F2E-4B1E-A7D4-61BC09B647B9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1523,54 +1526,54 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
@@ -1583,36 +1586,36 @@
         <v>3.76</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J2" s="8">
         <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
@@ -1625,36 +1628,36 @@
         <v>142.29</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J3" s="8">
         <v>0.5</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -1667,36 +1670,36 @@
         <v>53.58</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J4" s="8">
         <v>0.15</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
@@ -1709,36 +1712,36 @@
         <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J5" s="8">
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1">
         <v>30</v>
@@ -1751,36 +1754,36 @@
         <v>33</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J6" s="8">
         <v>1</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1">
         <v>30</v>
@@ -1793,36 +1796,36 @@
         <v>383.09999999999997</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J7" s="8">
         <v>1</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1835,36 +1838,36 @@
         <v>395</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J8" s="8">
         <v>0.7</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1877,36 +1880,36 @@
         <v>67.7</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J9" s="8">
         <v>0.5</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1919,36 +1922,36 @@
         <v>31.71</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J10" s="8">
         <v>0.15</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1961,36 +1964,36 @@
         <v>399</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J11" s="8">
         <v>0.7</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -2003,36 +2006,36 @@
         <v>47.43</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J12" s="8">
         <v>0.5</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -2045,36 +2048,36 @@
         <v>17.86</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J13" s="8">
         <v>0.15</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -2087,36 +2090,36 @@
         <v>65.53</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="8">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J14" s="8">
-        <v>1</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="B15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -2129,36 +2132,36 @@
         <v>146.75</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J15" s="8">
         <v>1</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D16" s="1">
         <v>30</v>
@@ -2171,36 +2174,36 @@
         <v>44.1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J16" s="8">
         <v>0.25</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="D17" s="1">
         <v>30</v>
@@ -2213,36 +2216,36 @@
         <v>12</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J17" s="8">
         <v>1</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1">
         <v>30</v>
@@ -2255,36 +2258,36 @@
         <v>18.3</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J18" s="8">
         <v>1</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1">
         <v>4</v>
@@ -2297,36 +2300,36 @@
         <v>16</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J19" s="8">
         <v>1</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
@@ -2339,36 +2342,36 @@
         <v>16</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J20" s="8">
         <v>1</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
@@ -2381,36 +2384,36 @@
         <v>16</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J21" s="8">
         <v>1</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -2423,36 +2426,36 @@
         <v>16</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J22" s="8">
         <v>1</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
@@ -2465,36 +2468,36 @@
         <v>16</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J23" s="8">
         <v>1</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -2507,36 +2510,36 @@
         <v>16</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J24" s="8">
         <v>1</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="1">
         <v>4</v>
@@ -2549,36 +2552,36 @@
         <v>16</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" s="8">
+        <v>1</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J25" s="8">
-        <v>1</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="B26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1">
         <v>30</v>
@@ -2591,25 +2594,25 @@
         <v>12</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J26" s="8">
         <v>1</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2637,15 +2640,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -2653,7 +2656,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>20</v>
@@ -2661,22 +2664,22 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>30</v>
@@ -2684,7 +2687,7 @@
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -2692,7 +2695,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
@@ -2700,7 +2703,7 @@
     </row>
     <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>100</v>
@@ -2708,7 +2711,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2716,7 +2719,7 @@
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -2724,7 +2727,7 @@
     </row>
     <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
         <f>4*28</f>
@@ -2733,7 +2736,7 @@
     </row>
     <row r="14" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -2741,7 +2744,7 @@
     </row>
     <row r="15" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -2749,7 +2752,7 @@
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>5</v>
@@ -2765,7 +2768,7 @@
     </row>
     <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -2773,7 +2776,7 @@
     </row>
     <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -2781,7 +2784,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -2789,7 +2792,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -2797,7 +2800,7 @@
     </row>
     <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>10</v>
@@ -2805,7 +2808,7 @@
     </row>
     <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -2813,7 +2816,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <f>4*3+5</f>
@@ -2822,7 +2825,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>5</v>
@@ -2830,7 +2833,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
         <v>5</v>
@@ -2838,7 +2841,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -2846,7 +2849,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -2854,7 +2857,7 @@
     </row>
     <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="30" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -2870,7 +2873,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1">
         <v>4</v>
@@ -2878,7 +2881,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -2905,15 +2908,15 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>77.099999999999994</v>
@@ -2921,7 +2924,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>33</v>
@@ -2929,7 +2932,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>44.1</v>
@@ -2937,7 +2940,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>272.41999999999996</v>
@@ -2945,7 +2948,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>67.7</v>
@@ -2953,7 +2956,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>47.43</v>
@@ -2961,7 +2964,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>142.29</v>
@@ -2969,7 +2972,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -2977,7 +2980,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B12">
         <v>625.67999999999984</v>
@@ -2989,7 +2992,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>383.09999999999997</v>
@@ -2997,7 +3000,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>146.75</v>
@@ -3005,7 +3008,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>65.53</v>
@@ -3013,7 +3016,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16">
         <v>18.3</v>
@@ -3021,7 +3024,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -3029,7 +3032,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>909.76</v>
@@ -3037,7 +3040,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>3.76</v>
@@ -3045,7 +3048,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>395</v>
@@ -3053,7 +3056,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>399</v>
@@ -3061,7 +3064,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>16</v>
@@ -3069,7 +3072,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -3077,7 +3080,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -3085,7 +3088,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -3093,7 +3096,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26">
         <v>16</v>
@@ -3101,7 +3104,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>16</v>
@@ -3109,7 +3112,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -3117,7 +3120,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B29">
         <v>115.15</v>
@@ -3125,7 +3128,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>31.71</v>
@@ -3133,7 +3136,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31">
         <v>17.86</v>
@@ -3141,7 +3144,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32">
         <v>53.58</v>
@@ -3149,7 +3152,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>12</v>
@@ -3157,7 +3160,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B34">
         <v>2000.1099999999997</v>

</xml_diff>